<commit_message>
fix: - controles y consultas de A a BS se cambian algunas filas      - se incorpora valor desde A04 de controles/consultas de educadora de parvulo a BS en otros profesionales
</commit_message>
<xml_diff>
--- a/RECIBIDO/rx05.xlsx
+++ b/RECIBIDO/rx05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26924"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Respaldo Pc\Rayos 2023\2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pie diabético\Desktop\Main\ESTADISTICAS\SERIES_A\2025\05\RECIBIDO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F55CE1-79DC-4D44-81E4-695B423E5E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A76C90-F07F-46F6-95D5-72CCEFEB0B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30360" yWindow="720" windowWidth="21795" windowHeight="15480" tabRatio="624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="624" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>EXÁMENES RADIOLÓGICOS SIMPLES</t>
   </si>
@@ -142,6 +142,90 @@
   </si>
   <si>
     <t>Mayo</t>
+  </si>
+  <si>
+    <t>0401002</t>
+  </si>
+  <si>
+    <t>0401009</t>
+  </si>
+  <si>
+    <t>0401070</t>
+  </si>
+  <si>
+    <t>0401013</t>
+  </si>
+  <si>
+    <t>0401014</t>
+  </si>
+  <si>
+    <t>0401031</t>
+  </si>
+  <si>
+    <t>0401032</t>
+  </si>
+  <si>
+    <t>0401033</t>
+  </si>
+  <si>
+    <t>0401042</t>
+  </si>
+  <si>
+    <t>0401043</t>
+  </si>
+  <si>
+    <t>0401044</t>
+  </si>
+  <si>
+    <t>0401045</t>
+  </si>
+  <si>
+    <t>0401046</t>
+  </si>
+  <si>
+    <t>0401047</t>
+  </si>
+  <si>
+    <t>0401048</t>
+  </si>
+  <si>
+    <t>0401051</t>
+  </si>
+  <si>
+    <t>0401151</t>
+  </si>
+  <si>
+    <t>0401052</t>
+  </si>
+  <si>
+    <t>0401053</t>
+  </si>
+  <si>
+    <t>0401054</t>
+  </si>
+  <si>
+    <t>0401055</t>
+  </si>
+  <si>
+    <t>0401056</t>
+  </si>
+  <si>
+    <t>0401057</t>
+  </si>
+  <si>
+    <t>0401058</t>
+  </si>
+  <si>
+    <t>0401059</t>
+  </si>
+  <si>
+    <t>0401060</t>
+  </si>
+  <si>
+    <t>0401062</t>
+  </si>
+  <si>
+    <t>0401063</t>
   </si>
 </sst>
 </file>
@@ -563,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -613,14 +697,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -661,6 +740,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -973,18 +1058,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Hoja1">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="115.85546875" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -994,32 +1079,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
-      <c r="G1" s="35"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="36">
+      <c r="A2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="33">
         <v>2025</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="37"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="31"/>
-      <c r="B3" s="32"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
@@ -1037,10 +1122,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="17">
-        <v>401002</v>
-      </c>
-      <c r="B4" s="18" t="s">
+      <c r="A4" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3"/>
@@ -1049,16 +1134,16 @@
         <v>1</v>
       </c>
       <c r="F4" s="5"/>
-      <c r="G4" s="28">
+      <c r="G4" s="25">
         <f>SUM(C4:F4)</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>401009</v>
-      </c>
-      <c r="B5" s="18" t="s">
+      <c r="A5" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1">
@@ -1073,7 +1158,7 @@
       <c r="F5" s="7">
         <v>5</v>
       </c>
-      <c r="G5" s="28">
+      <c r="G5" s="25">
         <f t="shared" ref="G5:G32" si="0">SUM(C5:F5)</f>
         <v>48</v>
       </c>
@@ -1081,10 +1166,10 @@
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>401070</v>
-      </c>
-      <c r="B6" s="18" t="s">
+      <c r="A6" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="1">
@@ -1099,7 +1184,7 @@
       <c r="F6" s="8">
         <v>9</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="25">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
@@ -1107,8 +1192,8 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="18" t="s">
+      <c r="A7" s="36"/>
+      <c r="B7" s="17" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="1">
@@ -1123,17 +1208,17 @@
       <c r="F7" s="5">
         <v>3</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="25">
         <f t="shared" si="0"/>
         <v>108</v>
       </c>
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="17">
-        <v>401013</v>
-      </c>
-      <c r="B8" s="18" t="s">
+      <c r="A8" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1">
@@ -1144,17 +1229,17 @@
         <v>2</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="28">
+      <c r="G8" s="25">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="I8" s="5"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
-        <v>401014</v>
-      </c>
-      <c r="B9" s="18" t="s">
+      <c r="A9" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1">
@@ -1165,17 +1250,17 @@
         <v>2</v>
       </c>
       <c r="F9" s="8"/>
-      <c r="G9" s="28">
+      <c r="G9" s="25">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>401031</v>
-      </c>
-      <c r="B10" s="18" t="s">
+      <c r="A10" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1">
@@ -1186,17 +1271,17 @@
         <v>2</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="28">
+      <c r="G10" s="25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
-        <v>401032</v>
-      </c>
-      <c r="B11" s="20" t="s">
+      <c r="A11" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="2">
@@ -1207,34 +1292,34 @@
         <v>1</v>
       </c>
       <c r="F11" s="9"/>
-      <c r="G11" s="28">
+      <c r="G11" s="25">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>401033</v>
-      </c>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="5"/>
-      <c r="G12" s="28">
+      <c r="G12" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I12" s="5"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="17">
-        <v>401042</v>
-      </c>
-      <c r="B13" s="21" t="s">
+      <c r="A13" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="2">
@@ -1247,51 +1332,51 @@
       <c r="F13" s="9">
         <v>1</v>
       </c>
-      <c r="G13" s="28">
+      <c r="G13" s="25">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
-        <v>401043</v>
-      </c>
-      <c r="B14" s="20" t="s">
+      <c r="A14" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="5"/>
-      <c r="G14" s="28">
+      <c r="G14" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
-        <v>401044</v>
-      </c>
-      <c r="B15" s="21" t="s">
+      <c r="A15" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="19" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="9"/>
-      <c r="G15" s="28">
+      <c r="G15" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
-        <v>401045</v>
-      </c>
-      <c r="B16" s="20" t="s">
+      <c r="A16" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="18" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="3">
@@ -1304,7 +1389,7 @@
       <c r="F16" s="5">
         <v>2</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="25">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
@@ -1312,10 +1397,10 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
-        <v>401046</v>
-      </c>
-      <c r="B17" s="21" t="s">
+      <c r="A17" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="19" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="2">
@@ -1328,7 +1413,7 @@
       <c r="F17" s="9">
         <v>8</v>
       </c>
-      <c r="G17" s="28">
+      <c r="G17" s="25">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
@@ -1336,44 +1421,44 @@
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
-        <v>401047</v>
-      </c>
-      <c r="B18" s="20" t="s">
+      <c r="A18" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="28">
+      <c r="G18" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
-        <v>401048</v>
-      </c>
-      <c r="B19" s="21" t="s">
+      <c r="A19" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="28">
+      <c r="G19" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
-        <v>401051</v>
-      </c>
-      <c r="B20" s="20" t="s">
+      <c r="A20" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="3">
@@ -1386,7 +1471,7 @@
       <c r="F20" s="5">
         <v>14</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="25">
         <f t="shared" si="0"/>
         <v>69</v>
       </c>
@@ -1394,10 +1479,10 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
-        <v>401151</v>
-      </c>
-      <c r="B21" s="21" t="s">
+      <c r="A21" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="2"/>
@@ -1406,16 +1491,16 @@
         <v>0</v>
       </c>
       <c r="F21" s="9"/>
-      <c r="G21" s="28">
+      <c r="G21" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
-        <v>401052</v>
-      </c>
-      <c r="B22" s="20" t="s">
+      <c r="A22" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C22" s="3">
@@ -1428,17 +1513,17 @@
       <c r="F22" s="5">
         <v>5</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="25">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
-        <v>401053</v>
-      </c>
-      <c r="B23" s="21" t="s">
+      <c r="A23" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="2">
@@ -1449,17 +1534,17 @@
         <v>2</v>
       </c>
       <c r="F23" s="9"/>
-      <c r="G23" s="28">
+      <c r="G23" s="25">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
-        <v>401054</v>
-      </c>
-      <c r="B24" s="20" t="s">
+      <c r="A24" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="4">
@@ -1474,7 +1559,7 @@
       <c r="F24" s="10">
         <v>7</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="25">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
@@ -1482,10 +1567,10 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
-        <v>401055</v>
-      </c>
-      <c r="B25" s="18" t="s">
+      <c r="A25" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="1">
@@ -1494,66 +1579,66 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="5"/>
-      <c r="G25" s="28">
+      <c r="G25" s="25">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
-        <v>401056</v>
-      </c>
-      <c r="B26" s="18" t="s">
+      <c r="A26" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="7"/>
-      <c r="G26" s="28">
+      <c r="G26" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
-        <v>401057</v>
-      </c>
-      <c r="B27" s="18" t="s">
+      <c r="A27" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="8"/>
-      <c r="G27" s="28">
+      <c r="G27" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
-        <v>401058</v>
-      </c>
-      <c r="B28" s="18" t="s">
+      <c r="A28" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="8"/>
-      <c r="G28" s="28">
+      <c r="G28" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
-        <v>401059</v>
-      </c>
-      <c r="B29" s="18" t="s">
+      <c r="A29" s="35" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="1">
@@ -1566,7 +1651,7 @@
       <c r="F29" s="5">
         <v>2</v>
       </c>
-      <c r="G29" s="28">
+      <c r="G29" s="25">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
@@ -1574,10 +1659,10 @@
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
-        <v>401060</v>
-      </c>
-      <c r="B30" s="18" t="s">
+      <c r="A30" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>32</v>
       </c>
       <c r="C30" s="1">
@@ -1592,7 +1677,7 @@
       <c r="F30" s="8">
         <v>13</v>
       </c>
-      <c r="G30" s="28">
+      <c r="G30" s="25">
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
@@ -1600,10 +1685,10 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
-        <v>401062</v>
-      </c>
-      <c r="B31" s="18" t="s">
+      <c r="A31" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>35</v>
       </c>
       <c r="C31" s="1">
@@ -1616,7 +1701,7 @@
       <c r="F31" s="5">
         <v>1</v>
       </c>
-      <c r="G31" s="28">
+      <c r="G31" s="25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
@@ -1624,17 +1709,17 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
-        <v>401063</v>
-      </c>
-      <c r="B32" s="18" t="s">
+      <c r="A32" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="8"/>
-      <c r="G32" s="28">
+      <c r="G32" s="25">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1642,14 +1727,14 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="24"/>
-      <c r="B33" s="23"/>
+      <c r="A33" s="21"/>
+      <c r="B33" s="20"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="26" t="s">
+      <c r="D33" s="22"/>
+      <c r="E33" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="27"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="12">
         <f>SUM(G4:G32)</f>
         <v>686</v>

</xml_diff>